<commit_message>
UCID updated (Update Profile)
</commit_message>
<xml_diff>
--- a/Iteration 2 docs/UCID Table (updated).xlsx
+++ b/Iteration 2 docs/UCID Table (updated).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaura\Downloads\CarRental\Iteration 2 docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7D8A70-ED2C-4D98-8509-737E10D3DFEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD045EE-7EEA-4941-A3DB-A305F0F45214}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -169,9 +169,6 @@
 Club Membership (User only)</t>
   </si>
   <si>
-    <t>System user indicates that he wants to modify the System User profile while viewing it (Admin is not allowed to modify). This function is performed after View Profile function. Output is updated after a confirmation message.</t>
-  </si>
-  <si>
     <t>Search Vehicles</t>
   </si>
   <si>
@@ -560,6 +557,30 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> the selected user's profile. The output is updated after a confirmation message. Function is performed after View User function.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">System user indicates that he wants to modify the System User profile while viewing it (Admin is not allowed to modify). This function is performed after View Profile function. Output is updated after a confirmation message </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and the user is shown a successful toast message</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
     </r>
   </si>
 </sst>
@@ -1628,9 +1649,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="A1:H24"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="99" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1798,7 +1819,7 @@
         <v>23</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>29</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" ht="163.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1806,25 +1827,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="D7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="E7" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="F7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="G7" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="H7" s="11" t="s">
         <v>35</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" ht="184.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1832,25 +1853,25 @@
         <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>37</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>38</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="H8" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="145.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1858,25 +1879,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>42</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="H9" s="12" t="s">
         <v>45</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1" ht="129.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1884,25 +1905,25 @@
         <v>9</v>
       </c>
       <c r="B10" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="11" t="s">
+      <c r="E10" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="F10" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="G10" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="H10" s="11" t="s">
         <v>51</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="5" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
@@ -1910,25 +1931,25 @@
         <v>10</v>
       </c>
       <c r="B11" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>53</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>54</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="H11" s="12" t="s">
         <v>56</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="5" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
@@ -1936,25 +1957,25 @@
         <v>11</v>
       </c>
       <c r="B12" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="14" t="s">
         <v>58</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>59</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G12" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="H12" s="12" t="s">
         <v>60</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -1962,25 +1983,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="16" t="s">
-        <v>63</v>
-      </c>
       <c r="D13" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="11" t="s">
         <v>64</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -1988,25 +2009,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="D14" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="E14" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="F14" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="G14" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="H14" s="19" t="s">
         <v>71</v>
-      </c>
-      <c r="H14" s="19" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="201.6" x14ac:dyDescent="0.3">
@@ -2014,25 +2035,25 @@
         <v>14</v>
       </c>
       <c r="B15" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>73</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>74</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="H15" s="11" t="s">
         <v>76</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="201.6" x14ac:dyDescent="0.3">
@@ -2040,25 +2061,25 @@
         <v>15</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F16" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="G16" s="11" t="s">
-        <v>76</v>
-      </c>
       <c r="H16" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="6" customFormat="1" ht="201.6" x14ac:dyDescent="0.3">
@@ -2066,25 +2087,25 @@
         <v>16</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E17" s="22" t="s">
         <v>12</v>
       </c>
       <c r="F17" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="G17" s="22" t="s">
-        <v>76</v>
-      </c>
       <c r="H17" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="6" customFormat="1" ht="201.6" x14ac:dyDescent="0.3">
@@ -2092,25 +2113,25 @@
         <v>17</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E18" s="22" t="s">
         <v>12</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G18" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="H18" s="22" t="s">
         <v>83</v>
-      </c>
-      <c r="H18" s="22" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="1" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
@@ -2118,25 +2139,25 @@
         <v>16</v>
       </c>
       <c r="B19" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="D19" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="E19" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="F19" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="G19" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="H19" s="11" t="s">
         <v>90</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="230.4" x14ac:dyDescent="0.3">
@@ -2144,25 +2165,25 @@
         <v>17</v>
       </c>
       <c r="B20" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>92</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>93</v>
       </c>
       <c r="E20" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F20" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="G20" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="H20" s="11" t="s">
         <v>95</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -2170,25 +2191,25 @@
         <v>18</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E21" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F21" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="G21" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="H21" s="11" t="s">
         <v>99</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
@@ -2196,25 +2217,25 @@
         <v>19</v>
       </c>
       <c r="B22" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" s="11" t="s">
+      <c r="F22" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="G22" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="G22" s="13" t="s">
+      <c r="H22" s="11" t="s">
         <v>104</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
@@ -2222,25 +2243,25 @@
         <v>20</v>
       </c>
       <c r="B23" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="E23" s="24" t="s">
+      <c r="F23" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="G23" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="G23" s="12" t="s">
+      <c r="H23" s="12" t="s">
         <v>109</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
@@ -2248,25 +2269,25 @@
         <v>21</v>
       </c>
       <c r="B24" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="11" t="s">
         <v>111</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>112</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F24" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="G24" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="H24" s="11" t="s">
         <v>114</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -2309,7 +2330,8 @@
     <sortCondition ref="A2:A20"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2353,57 +2375,57 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DB schema updated, Minor function update in UCID and started functionality for SearchVehicle
</commit_message>
<xml_diff>
--- a/Iteration 2 docs/UCID Table (updated).xlsx
+++ b/Iteration 2 docs/UCID Table (updated).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaura\Downloads\CarRental\Iteration 2 docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD045EE-7EEA-4941-A3DB-A305F0F45214}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8213EBC8-2EDB-4325-A5AC-5EEC34F2F2AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -195,10 +195,6 @@
 (User may also navigate back to User homescreen)</t>
   </si>
   <si>
-    <t xml:space="preserve">Output produced is a selectable list of cars available to view which will be displayed as per requested occupant capacity. Output is sorted by cost (lowest to highest) then by date/time in chronological order. Total cost shown does not include options only basic car fees plus tax. This function shall not allow the User to request a vehicle if his rental status has been revoked.
-</t>
-  </si>
-  <si>
     <t>Select Vehicle</t>
   </si>
   <si>
@@ -581,6 +577,43 @@
         <scheme val="minor"/>
       </rPr>
       <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Output produced is a selectable list of cars available to view which will be displayed as per requested occupant capacity. Output is sorted by cost (lowest to highest) </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then by date/time in chronological orde</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Total cost shown does not include options only basic car fees plus tax. This function shall not allow the User to request a vehicle if his rental status has been revoked.
+</t>
     </r>
   </si>
 </sst>
@@ -1650,8 +1683,8 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="99" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1819,7 +1852,7 @@
         <v>23</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" ht="163.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1845,7 +1878,7 @@
         <v>34</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>35</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" ht="184.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1853,25 +1886,25 @@
         <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>30</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="H8" s="11" t="s">
         <v>39</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="145.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1879,25 +1912,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>30</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="H9" s="12" t="s">
         <v>44</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1" ht="129.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1905,25 +1938,25 @@
         <v>9</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="F10" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="G10" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="H10" s="11" t="s">
         <v>50</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="5" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
@@ -1931,25 +1964,25 @@
         <v>10</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>30</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="H11" s="12" t="s">
         <v>55</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="5" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
@@ -1957,25 +1990,25 @@
         <v>11</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>30</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G12" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" s="12" t="s">
         <v>59</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -1983,25 +2016,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="16" t="s">
-        <v>62</v>
-      </c>
       <c r="D13" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="11" t="s">
         <v>63</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -2009,25 +2042,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="D14" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="E14" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="F14" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="G14" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="H14" s="19" t="s">
         <v>70</v>
-      </c>
-      <c r="H14" s="19" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="201.6" x14ac:dyDescent="0.3">
@@ -2035,25 +2068,25 @@
         <v>14</v>
       </c>
       <c r="B15" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>72</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>73</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="H15" s="11" t="s">
         <v>75</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="201.6" x14ac:dyDescent="0.3">
@@ -2061,25 +2094,25 @@
         <v>15</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F16" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="G16" s="11" t="s">
-        <v>75</v>
-      </c>
       <c r="H16" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="6" customFormat="1" ht="201.6" x14ac:dyDescent="0.3">
@@ -2087,25 +2120,25 @@
         <v>16</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E17" s="22" t="s">
         <v>12</v>
       </c>
       <c r="F17" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="G17" s="22" t="s">
-        <v>75</v>
-      </c>
       <c r="H17" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="6" customFormat="1" ht="201.6" x14ac:dyDescent="0.3">
@@ -2113,25 +2146,25 @@
         <v>17</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E18" s="22" t="s">
         <v>12</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G18" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="H18" s="22" t="s">
         <v>82</v>
-      </c>
-      <c r="H18" s="22" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="1" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
@@ -2139,25 +2172,25 @@
         <v>16</v>
       </c>
       <c r="B19" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="D19" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="E19" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="F19" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="G19" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="H19" s="11" t="s">
         <v>89</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="230.4" x14ac:dyDescent="0.3">
@@ -2165,25 +2198,25 @@
         <v>17</v>
       </c>
       <c r="B20" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>91</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>92</v>
       </c>
       <c r="E20" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F20" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G20" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="H20" s="11" t="s">
         <v>94</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -2191,25 +2224,25 @@
         <v>18</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E21" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F21" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G21" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="H21" s="11" t="s">
         <v>98</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
@@ -2217,25 +2250,25 @@
         <v>19</v>
       </c>
       <c r="B22" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E22" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E22" s="11" t="s">
+      <c r="F22" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="G22" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="G22" s="13" t="s">
+      <c r="H22" s="11" t="s">
         <v>103</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
@@ -2243,25 +2276,25 @@
         <v>20</v>
       </c>
       <c r="B23" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="E23" s="24" t="s">
+      <c r="F23" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="G23" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="G23" s="12" t="s">
+      <c r="H23" s="12" t="s">
         <v>108</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
@@ -2269,25 +2302,25 @@
         <v>21</v>
       </c>
       <c r="B24" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="11" t="s">
         <v>110</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>111</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F24" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="G24" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="H24" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -2380,52 +2413,52 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Third Party library added-Joda Time, Minor changes in UCID, Added ViewSelectedVehicle screen and some functionality, DB Schema changed, Some minor code changes here and there.
</commit_message>
<xml_diff>
--- a/Iteration 2 docs/UCID Table (updated).xlsx
+++ b/Iteration 2 docs/UCID Table (updated).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaura\Downloads\CarRental\Iteration 2 docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8213EBC8-2EDB-4325-A5AC-5EEC34F2F2AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F514D797-A408-4557-BE50-8F50438E323A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="119">
   <si>
     <t>Function Number</t>
   </si>
@@ -201,27 +201,10 @@
     <t>Search Vehicles Screen</t>
   </si>
   <si>
-    <t xml:space="preserve">Car Number
-Car Name
-Car Occupant Capacity
-Start Date
-Start Time
-End Date
-End Time
-Total Cost
-GPS selected
-Sirius selected
-OnStar selected
-</t>
-  </si>
-  <si>
     <t>Selected Vehicle Screen
 (User may also navigate back to Search Vehicles Screen or User homescreen)</t>
   </si>
   <si>
-    <t>Output is the details of the selected car from the list. Function is performed after Search Vehicles function. The User can make a reservation from this output.</t>
-  </si>
-  <si>
     <t>Reserve Rental</t>
   </si>
   <si>
@@ -234,9 +217,6 @@
   <si>
     <t>Reserve Summary screen
 (User may also navigate back to User homescreen)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">System user can book the vehicle by selecting the "Reserve" option. The total cost shall be updated to reflect the selected options. This function allows the user to finalize the reservation after the Select Vehicle function. The reservation number is the success message indicating the reservation was successful.  </t>
   </si>
   <si>
     <t>View Rental History</t>
@@ -614,6 +594,106 @@
       </rPr>
       <t xml:space="preserve">. Total cost shown does not include options only basic car fees plus tax. This function shall not allow the User to request a vehicle if his rental status has been revoked.
 </t>
+    </r>
+  </si>
+  <si>
+    <t>View Selected Vehicle</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Car Number
+Car Name
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Selected Occupant Capacity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Start Date
+Start Time
+End Date
+End Time
+Total Cost
+GPS selected
+Sirius selected
+OnStar selected
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>System user can book the vehicle by selecting the "Reserve" option.</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> The total cost shall be updated to reflect the selected options</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> This function allows the user to finalize the reservation after the Select Vehicle function. The reservation number is the success message indicating the reservation was successful.  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Output is the details of the selected car from the list. Function is performed after Search Vehicles function. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The total cost shall be updated to reflect the selected options. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The User can make a reservation from this output.</t>
     </r>
   </si>
 </sst>
@@ -1684,7 +1764,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="99" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1852,7 +1932,7 @@
         <v>23</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" ht="163.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1878,15 +1958,15 @@
         <v>34</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" ht="184.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>7</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>35</v>
+      <c r="B8" s="21" t="s">
+        <v>115</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>30</v>
@@ -1898,13 +1978,13 @@
         <v>12</v>
       </c>
       <c r="F8" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="G8" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="11" t="s">
-        <v>38</v>
-      </c>
       <c r="H8" s="11" t="s">
-        <v>39</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="145.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1912,25 +1992,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>30</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1" ht="129.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1938,25 +2018,25 @@
         <v>9</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="H10" s="11" t="s">
         <v>47</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="5" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
@@ -1964,25 +2044,25 @@
         <v>10</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>30</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="5" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
@@ -1990,25 +2070,25 @@
         <v>11</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>30</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -2016,25 +2096,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -2042,25 +2122,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="F14" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="G14" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="H14" s="19" t="s">
         <v>67</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="H14" s="19" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="201.6" x14ac:dyDescent="0.3">
@@ -2068,25 +2148,25 @@
         <v>14</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="201.6" x14ac:dyDescent="0.3">
@@ -2094,25 +2174,25 @@
         <v>15</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="6" customFormat="1" ht="201.6" x14ac:dyDescent="0.3">
@@ -2120,25 +2200,25 @@
         <v>16</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E17" s="22" t="s">
         <v>12</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G17" s="22" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H17" s="22" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="6" customFormat="1" ht="201.6" x14ac:dyDescent="0.3">
@@ -2146,25 +2226,25 @@
         <v>17</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E18" s="22" t="s">
         <v>12</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G18" s="22" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H18" s="22" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="1" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
@@ -2172,25 +2252,25 @@
         <v>16</v>
       </c>
       <c r="B19" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="F19" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="G19" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="H19" s="11" t="s">
         <v>86</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="230.4" x14ac:dyDescent="0.3">
@@ -2198,25 +2278,25 @@
         <v>17</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E20" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -2224,25 +2304,25 @@
         <v>18</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E21" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
@@ -2250,25 +2330,25 @@
         <v>19</v>
       </c>
       <c r="B22" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="G22" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E22" s="11" t="s">
+      <c r="H22" s="11" t="s">
         <v>100</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
@@ -2276,25 +2356,25 @@
         <v>20</v>
       </c>
       <c r="B23" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="G23" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="E23" s="24" t="s">
+      <c r="H23" s="12" t="s">
         <v>105</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
@@ -2302,25 +2382,25 @@
         <v>21</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -2418,47 +2498,47 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
VIEW AVAILABLE CARS FUNCTIONALITY COMPLETED
</commit_message>
<xml_diff>
--- a/Iteration 2 docs/UCID Table (updated).xlsx
+++ b/Iteration 2 docs/UCID Table (updated).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaura\Downloads\CarRental\Iteration 2 docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeevesh Sehgal\Desktop\Latest Car\Iteration 2 docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F514D797-A408-4557-BE50-8F50438E323A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D6BBAB-E3F2-4858-8366-7B51A064A4EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1763,8 +1763,8 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="99" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Removed the car status attribute for search car
</commit_message>
<xml_diff>
--- a/Iteration 2 docs/UCID Table (updated).xlsx
+++ b/Iteration 2 docs/UCID Table (updated).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeevesh Sehgal\Desktop\Latest Car\Iteration 2 docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D6BBAB-E3F2-4858-8366-7B51A064A4EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC06D90E-E461-4D6A-9481-3F25CAE4FDEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -451,14 +451,6 @@
 End Time (default=Now + 1 hour)</t>
   </si>
   <si>
-    <t xml:space="preserve">Car Name
-Car Number
-Car Occupant Capacity
-Cost Per Day
-Car Reservation status
-</t>
-  </si>
-  <si>
     <t>View Available Cars Screen (Rental Manager can navigate back to Rental Manager homescreen or his homescreen)</t>
   </si>
   <si>
@@ -489,17 +481,6 @@
   </si>
   <si>
     <t>View Available Cars Screen</t>
-  </si>
-  <si>
-    <t>Car Name
-Car Capacity
-Weekday Rate
-Weekend Rate
-Week Rate
-GPS rate
-OnStar rate
-SiriusXM rate
-Car status</t>
   </si>
   <si>
     <t>View Car Details Screen (Rental Manager can navigate back to View Available Car screen or rental homescreen)</t>
@@ -557,43 +538,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Output produced is a selectable list of cars available to view which will be displayed as per requested occupant capacity. Output is sorted by cost (lowest to highest) </t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>then by date/time in chronological orde</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. Total cost shown does not include options only basic car fees plus tax. This function shall not allow the User to request a vehicle if his rental status has been revoked.
-</t>
     </r>
   </si>
   <si>
@@ -694,6 +638,86 @@
         <scheme val="minor"/>
       </rPr>
       <t>The User can make a reservation from this output.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Car Name
+Car Capacity
+Weekday Rate
+Weekend Rate
+Week Rate
+GPS rate
+OnStar rate
+SiriusXM rate
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Car status</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Output produced is a selectable list of cars available to view which will be displayed as per requested occupant capacity. Output is sorted by cost (lowest to highest) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>then by date/time in chronological order</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Total cost shown does not include options only basic car fees plus tax. This function shall not allow the User to request a vehicle if his rental status has been revoked.
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Car Name
+Car Number
+Car Occupant Capacity
+Cost Per Day
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Car Status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
     </r>
   </si>
 </sst>
@@ -1763,8 +1787,8 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="99" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1932,7 +1956,7 @@
         <v>23</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="1" customFormat="1" ht="163.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1958,7 +1982,7 @@
         <v>34</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="1" customFormat="1" ht="184.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1966,7 +1990,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>30</v>
@@ -1978,13 +2002,13 @@
         <v>12</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>37</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="145.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -2010,7 +2034,7 @@
         <v>41</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="1" customFormat="1" ht="129.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2174,7 +2198,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>62</v>
@@ -2192,7 +2216,7 @@
         <v>71</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="6" customFormat="1" ht="201.6" x14ac:dyDescent="0.3">
@@ -2342,13 +2366,13 @@
         <v>97</v>
       </c>
       <c r="F22" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="G22" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="G22" s="13" t="s">
+      <c r="H22" s="11" t="s">
         <v>99</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
@@ -2356,7 +2380,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>81</v>
@@ -2365,16 +2389,16 @@
         <v>82</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F23" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="G23" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="G23" s="12" t="s">
+      <c r="H23" s="12" t="s">
         <v>104</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
@@ -2382,25 +2406,25 @@
         <v>21</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>81</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F24" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="H24" s="11" t="s">
         <v>108</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -2498,7 +2522,7 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
@@ -2538,7 +2562,7 @@
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>